<commit_message>
Updates to schedule and tasks
</commit_message>
<xml_diff>
--- a/planning/TASKS_CitizenData.xlsx
+++ b/planning/TASKS_CitizenData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Task</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>DueDate</t>
+  </si>
+  <si>
+    <t>Scheduled</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,11 +488,18 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="C3" t="str">
+        <f>TEXT(D3,"DD-MMM-YY")</f>
+        <v>15-Oct-19</v>
+      </c>
+      <c r="D3" s="5">
+        <v>43753</v>
+      </c>
+      <c r="E3" s="7">
+        <v>60</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" t="s">
         <v>6</v>

</xml_diff>